<commit_message>
🚀 [Auto] Sincronização de dados e código
</commit_message>
<xml_diff>
--- a/avaliacoes_garantia.xlsx
+++ b/avaliacoes_garantia.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,20 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" s="2" t="n">
+        <v>45895.62649680555</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NjMzNDFkZTQtNWEwYi00MGVhLWE0YTMtZDEzMmM1YjFjNmUyOjU3MDE2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>